<commit_message>
Si pintan rojo los suples que no se consideran en los planos
</commit_message>
<xml_diff>
--- a/Tarea 05/Armadura losas.xlsx
+++ b/Tarea 05/Armadura losas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignac\Google Drive (ignacio.yanez.g@ug.uchile.cl)\Universidad\Semestre 12 Primavera 2018\proyecto de hormigon\proyecto-CI5206\Tarea 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CE2DE2-1222-49D5-B3BC-AEC5E4F34ECE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524F8D02-0C76-4FDB-A3A8-79409D169FFB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="2" xr2:uid="{DCE08E2E-61A3-415E-97C5-889CEC2E68E5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="9" xr2:uid="{DCE08E2E-61A3-415E-97C5-889CEC2E68E5}"/>
   </bookViews>
   <sheets>
     <sheet name="tablas" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3066" uniqueCount="342">
   <si>
     <t>Caso</t>
   </si>
@@ -1517,6 +1517,99 @@
   <si>
     <t>Losa de Cubierta</t>
   </si>
+  <si>
+    <t xml:space="preserve">Interacciones entre losas </t>
+  </si>
+  <si>
+    <t>0130</t>
+  </si>
+  <si>
+    <t>0131</t>
+  </si>
+  <si>
+    <t>0132</t>
+  </si>
+  <si>
+    <t>0133</t>
+  </si>
+  <si>
+    <t>0134</t>
+  </si>
+  <si>
+    <t>0135</t>
+  </si>
+  <si>
+    <t>0136</t>
+  </si>
+  <si>
+    <t>0137</t>
+  </si>
+  <si>
+    <t>0138</t>
+  </si>
+  <si>
+    <t>0139</t>
+  </si>
+  <si>
+    <t>0140</t>
+  </si>
+  <si>
+    <t>0141</t>
+  </si>
+  <si>
+    <t>0142</t>
+  </si>
+  <si>
+    <t>0143</t>
+  </si>
+  <si>
+    <t>0144</t>
+  </si>
+  <si>
+    <t>0145</t>
+  </si>
+  <si>
+    <t>0146</t>
+  </si>
+  <si>
+    <t>0147</t>
+  </si>
+  <si>
+    <t>0148</t>
+  </si>
+  <si>
+    <t>0149</t>
+  </si>
+  <si>
+    <t>0150</t>
+  </si>
+  <si>
+    <t>0151</t>
+  </si>
+  <si>
+    <t>0152</t>
+  </si>
+  <si>
+    <t>0153</t>
+  </si>
+  <si>
+    <t>0154</t>
+  </si>
+  <si>
+    <t>0155</t>
+  </si>
+  <si>
+    <t>0156</t>
+  </si>
+  <si>
+    <t>0157</t>
+  </si>
+  <si>
+    <t>0158</t>
+  </si>
+  <si>
+    <t>Dif [\%]</t>
+  </si>
 </sst>
 </file>
 
@@ -1580,7 +1673,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1623,8 +1716,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1997,12 +2096,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2472,6 +2586,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7276,8 +7408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78345A7D-A1BA-45AA-A425-C9A5BA2365DA}">
   <dimension ref="B2:AD115"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82:X82"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L83" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC113" sqref="AC113:AD113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13544,11 +13676,11 @@
       <c r="B103" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="C103" s="149" t="str">
+      <c r="C103" s="181" t="str">
         <f>IF(C102&gt;$C$12,"φ"&amp;IF(VLOOKUP(VLOOKUP(C102,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(C102,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;C102,VLOOKUP(C102+0.1,tablas!$R$3:$T$66,2,TRUE),VLOOKUP(C102,tablas!$R$3:$T$66,2,TRUE))&amp;"@"&amp;IF(VLOOKUP(VLOOKUP(C102,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(C102,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;C102,VLOOKUP(C102+0.1,tablas!$R$3:$T$66,3,TRUE),VLOOKUP(C102,tablas!$R$3:$T$66,3,TRUE)),$C$13)</f>
         <v>φ8@17</v>
       </c>
-      <c r="D103" s="150"/>
+      <c r="D103" s="182"/>
       <c r="E103" s="149" t="str">
         <f>IF(E102&gt;$C$12,"φ"&amp;IF(VLOOKUP(VLOOKUP(E102,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(E102,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;E102,VLOOKUP(E102+0.1,tablas!$R$3:$T$66,2,TRUE),VLOOKUP(E102,tablas!$R$3:$T$66,2,TRUE))&amp;"@"&amp;IF(VLOOKUP(VLOOKUP(E102,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(E102,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;E102,VLOOKUP(E102+0.1,tablas!$R$3:$T$66,3,TRUE),VLOOKUP(E102,tablas!$R$3:$T$66,3,TRUE)),$C$13)</f>
         <v>φ8@17</v>
@@ -14694,8 +14826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5244357D-C98C-407F-BE7A-2CD9958ECD51}">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:L27"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18039,8 +18171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A607B1-B062-4618-98DA-7E7D42BE2ED5}">
   <dimension ref="B2:AF130"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView showGridLines="0" topLeftCell="L93" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W110" sqref="W110:X110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25431,11 +25563,11 @@
         <v>φ10@21</v>
       </c>
       <c r="V110" s="150"/>
-      <c r="W110" s="149" t="str">
+      <c r="W110" s="181" t="str">
         <f>IF(W109&gt;$C$12,"φ"&amp;IF(VLOOKUP(VLOOKUP(W109,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(W109,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;W109,VLOOKUP(W109+0.1,tablas!$R$3:$T$66,2,TRUE),VLOOKUP(W109,tablas!$R$3:$T$66,2,TRUE))&amp;"@"&amp;IF(VLOOKUP(VLOOKUP(W109,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(W109,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;W109,VLOOKUP(W109+0.1,tablas!$R$3:$T$66,3,TRUE),VLOOKUP(W109,tablas!$R$3:$T$66,3,TRUE)),$C$13)</f>
         <v>φ10@24</v>
       </c>
-      <c r="X110" s="150"/>
+      <c r="X110" s="182"/>
       <c r="Y110" s="149" t="str">
         <f>IF(Y109&gt;$C$12,"φ"&amp;IF(VLOOKUP(VLOOKUP(Y109,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(Y109,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;Y109,VLOOKUP(Y109+0.1,tablas!$R$3:$T$66,2,TRUE),VLOOKUP(Y109,tablas!$R$3:$T$66,2,TRUE))&amp;"@"&amp;IF(VLOOKUP(VLOOKUP(Y109,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(Y109,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;Y109,VLOOKUP(Y109+0.1,tablas!$R$3:$T$66,3,TRUE),VLOOKUP(Y109,tablas!$R$3:$T$66,3,TRUE)),$C$13)</f>
         <v>φ8@16</v>
@@ -27320,10 +27452,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45EDF2B-406A-4D1C-8D87-7AFA2BC4AA34}">
-  <dimension ref="B3:L37"/>
+  <dimension ref="B3:O100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:L8"/>
+    <sheetView showGridLines="0" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28268,7 +28400,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B33" s="125" t="s">
         <v>73</v>
       </c>
@@ -28304,7 +28436,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B34" s="125" t="s">
         <v>74</v>
       </c>
@@ -28340,7 +28472,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35" s="125" t="s">
         <v>75</v>
       </c>
@@ -28376,7 +28508,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B36" s="125" t="s">
         <v>76</v>
       </c>
@@ -28412,7 +28544,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="131" t="s">
         <v>77</v>
       </c>
@@ -28448,8 +28580,1215 @@
         <v>247</v>
       </c>
     </row>
+    <row r="41" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B41" s="179" t="s">
+        <v>311</v>
+      </c>
+      <c r="C41" s="179"/>
+      <c r="D41" s="180" t="s">
+        <v>341</v>
+      </c>
+      <c r="E41" s="180" t="s">
+        <v>112</v>
+      </c>
+      <c r="F41" s="180" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="180" t="s">
+        <v>98</v>
+      </c>
+      <c r="H41" s="180" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="180" t="s">
+        <v>113</v>
+      </c>
+      <c r="J41" s="177"/>
+      <c r="K41" s="177"/>
+      <c r="L41" s="177"/>
+      <c r="M41" s="177"/>
+      <c r="N41" s="177"/>
+      <c r="O41" s="177"/>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B42" s="178" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="178" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="177"/>
+      <c r="E42" s="177"/>
+      <c r="F42" s="177"/>
+      <c r="G42" s="177"/>
+      <c r="H42" s="177"/>
+      <c r="I42" s="177"/>
+      <c r="J42" s="177"/>
+      <c r="K42" s="177"/>
+      <c r="L42" s="177"/>
+      <c r="M42" s="177"/>
+      <c r="N42" s="177"/>
+      <c r="O42" s="177"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B43" s="178" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="178" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="177"/>
+      <c r="E43" s="177"/>
+      <c r="F43" s="177"/>
+      <c r="G43" s="177"/>
+      <c r="H43" s="177"/>
+      <c r="I43" s="177"/>
+      <c r="J43" s="177"/>
+      <c r="K43" s="177"/>
+      <c r="L43" s="177"/>
+      <c r="M43" s="177"/>
+      <c r="N43" s="177"/>
+      <c r="O43" s="177"/>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B44" s="178" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="178" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="177"/>
+      <c r="E44" s="177"/>
+      <c r="F44" s="177"/>
+      <c r="G44" s="177"/>
+      <c r="H44" s="177"/>
+      <c r="I44" s="177"/>
+      <c r="J44" s="177"/>
+      <c r="K44" s="177"/>
+      <c r="L44" s="177"/>
+      <c r="M44" s="177"/>
+      <c r="N44" s="177"/>
+      <c r="O44" s="177"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B45" s="178" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="178" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="177"/>
+      <c r="E45" s="177"/>
+      <c r="F45" s="177"/>
+      <c r="G45" s="177"/>
+      <c r="H45" s="177"/>
+      <c r="I45" s="177"/>
+      <c r="J45" s="177"/>
+      <c r="K45" s="177"/>
+      <c r="L45" s="177"/>
+      <c r="M45" s="177"/>
+      <c r="N45" s="177"/>
+      <c r="O45" s="177"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B46" s="178" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="178" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="177"/>
+      <c r="E46" s="177"/>
+      <c r="F46" s="177"/>
+      <c r="G46" s="177"/>
+      <c r="H46" s="177"/>
+      <c r="I46" s="177"/>
+      <c r="J46" s="177"/>
+      <c r="K46" s="177"/>
+      <c r="L46" s="177"/>
+      <c r="M46" s="177"/>
+      <c r="N46" s="177"/>
+      <c r="O46" s="177"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B47" s="178" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="178" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="177"/>
+      <c r="E47" s="177"/>
+      <c r="F47" s="177"/>
+      <c r="G47" s="177"/>
+      <c r="H47" s="177"/>
+      <c r="I47" s="177"/>
+      <c r="J47" s="177"/>
+      <c r="K47" s="177"/>
+      <c r="L47" s="177"/>
+      <c r="M47" s="177"/>
+      <c r="N47" s="177"/>
+      <c r="O47" s="177"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B48" s="178" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="178" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="177"/>
+      <c r="E48" s="177"/>
+      <c r="F48" s="177"/>
+      <c r="G48" s="177"/>
+      <c r="H48" s="177"/>
+      <c r="I48" s="177"/>
+      <c r="J48" s="177"/>
+      <c r="K48" s="177"/>
+      <c r="L48" s="177"/>
+      <c r="M48" s="177"/>
+      <c r="N48" s="177"/>
+      <c r="O48" s="177"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B49" s="178" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="178" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="177"/>
+      <c r="E49" s="177"/>
+      <c r="F49" s="177"/>
+      <c r="G49" s="177"/>
+      <c r="H49" s="177"/>
+      <c r="I49" s="177"/>
+      <c r="J49" s="177"/>
+      <c r="K49" s="177"/>
+      <c r="L49" s="177"/>
+      <c r="M49" s="177"/>
+      <c r="N49" s="177"/>
+      <c r="O49" s="177"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B50" s="178" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="178" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" s="177"/>
+      <c r="E50" s="177"/>
+      <c r="F50" s="177"/>
+      <c r="G50" s="177"/>
+      <c r="H50" s="177"/>
+      <c r="I50" s="177"/>
+      <c r="J50" s="177"/>
+      <c r="K50" s="177"/>
+      <c r="L50" s="177"/>
+      <c r="M50" s="177"/>
+      <c r="N50" s="177"/>
+      <c r="O50" s="177"/>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B51" s="178" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="178" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" s="177"/>
+      <c r="E51" s="177"/>
+      <c r="F51" s="177"/>
+      <c r="G51" s="177"/>
+      <c r="H51" s="177"/>
+      <c r="I51" s="177"/>
+      <c r="J51" s="177"/>
+      <c r="K51" s="177"/>
+      <c r="L51" s="177"/>
+      <c r="M51" s="177"/>
+      <c r="N51" s="177"/>
+      <c r="O51" s="177"/>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B52" s="178" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="178" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="177"/>
+      <c r="E52" s="177"/>
+      <c r="F52" s="177"/>
+      <c r="G52" s="177"/>
+      <c r="H52" s="177"/>
+      <c r="I52" s="177"/>
+      <c r="J52" s="177"/>
+      <c r="K52" s="177"/>
+      <c r="L52" s="177"/>
+      <c r="M52" s="177"/>
+      <c r="N52" s="177"/>
+      <c r="O52" s="177"/>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B53" s="178" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="178" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="177"/>
+      <c r="E53" s="177"/>
+      <c r="F53" s="177"/>
+      <c r="G53" s="177"/>
+      <c r="H53" s="177"/>
+      <c r="I53" s="177"/>
+      <c r="J53" s="177"/>
+      <c r="K53" s="177"/>
+      <c r="L53" s="177"/>
+      <c r="M53" s="177"/>
+      <c r="N53" s="177"/>
+      <c r="O53" s="177"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B54" s="178" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="178" t="s">
+        <v>61</v>
+      </c>
+      <c r="D54" s="177"/>
+      <c r="E54" s="177"/>
+      <c r="F54" s="177"/>
+      <c r="G54" s="177"/>
+      <c r="H54" s="177"/>
+      <c r="I54" s="177"/>
+      <c r="J54" s="177"/>
+      <c r="K54" s="177"/>
+      <c r="L54" s="177"/>
+      <c r="M54" s="177"/>
+      <c r="N54" s="177"/>
+      <c r="O54" s="177"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B55" s="178" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="178" t="s">
+        <v>62</v>
+      </c>
+      <c r="D55" s="177"/>
+      <c r="E55" s="177"/>
+      <c r="F55" s="177"/>
+      <c r="G55" s="177"/>
+      <c r="H55" s="177"/>
+      <c r="I55" s="177"/>
+      <c r="J55" s="177"/>
+      <c r="K55" s="177"/>
+      <c r="L55" s="177"/>
+      <c r="M55" s="177"/>
+      <c r="N55" s="177"/>
+      <c r="O55" s="177"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B56" s="178" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="178" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="177"/>
+      <c r="E56" s="177"/>
+      <c r="F56" s="177"/>
+      <c r="G56" s="177"/>
+      <c r="H56" s="177"/>
+      <c r="I56" s="177"/>
+      <c r="J56" s="177"/>
+      <c r="K56" s="177"/>
+      <c r="L56" s="177"/>
+      <c r="M56" s="177"/>
+      <c r="N56" s="177"/>
+      <c r="O56" s="177"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B57" s="178" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="178" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" s="177"/>
+      <c r="E57" s="177"/>
+      <c r="F57" s="177"/>
+      <c r="G57" s="177"/>
+      <c r="H57" s="177"/>
+      <c r="I57" s="177"/>
+      <c r="J57" s="177"/>
+      <c r="K57" s="177"/>
+      <c r="L57" s="177"/>
+      <c r="M57" s="177"/>
+      <c r="N57" s="177"/>
+      <c r="O57" s="177"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B58" s="178" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="178" t="s">
+        <v>65</v>
+      </c>
+      <c r="D58" s="177"/>
+      <c r="E58" s="177"/>
+      <c r="F58" s="177"/>
+      <c r="G58" s="177"/>
+      <c r="H58" s="177"/>
+      <c r="I58" s="177"/>
+      <c r="J58" s="177"/>
+      <c r="K58" s="177"/>
+      <c r="L58" s="177"/>
+      <c r="M58" s="177"/>
+      <c r="N58" s="177"/>
+      <c r="O58" s="177"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B59" s="178" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59" s="178" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" s="177"/>
+      <c r="E59" s="177"/>
+      <c r="F59" s="177"/>
+      <c r="G59" s="177"/>
+      <c r="H59" s="177"/>
+      <c r="I59" s="177"/>
+      <c r="J59" s="177"/>
+      <c r="K59" s="177"/>
+      <c r="L59" s="177"/>
+      <c r="M59" s="177"/>
+      <c r="N59" s="177"/>
+      <c r="O59" s="177"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B60" s="178" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" s="178" t="s">
+        <v>67</v>
+      </c>
+      <c r="D60" s="177"/>
+      <c r="E60" s="177"/>
+      <c r="F60" s="177"/>
+      <c r="G60" s="177"/>
+      <c r="H60" s="177"/>
+      <c r="I60" s="177"/>
+      <c r="J60" s="177"/>
+      <c r="K60" s="177"/>
+      <c r="L60" s="177"/>
+      <c r="M60" s="177"/>
+      <c r="N60" s="177"/>
+      <c r="O60" s="177"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B61" s="178" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="178" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" s="177"/>
+      <c r="E61" s="177"/>
+      <c r="F61" s="177"/>
+      <c r="G61" s="177"/>
+      <c r="H61" s="177"/>
+      <c r="I61" s="177"/>
+      <c r="J61" s="177"/>
+      <c r="K61" s="177"/>
+      <c r="L61" s="177"/>
+      <c r="M61" s="177"/>
+      <c r="N61" s="177"/>
+      <c r="O61" s="177"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B62" s="178" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="178" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" s="177"/>
+      <c r="E62" s="177"/>
+      <c r="F62" s="177"/>
+      <c r="G62" s="177"/>
+      <c r="H62" s="177"/>
+      <c r="I62" s="177"/>
+      <c r="J62" s="177"/>
+      <c r="K62" s="177"/>
+      <c r="L62" s="177"/>
+      <c r="M62" s="177"/>
+      <c r="N62" s="177"/>
+      <c r="O62" s="177"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B63" s="178" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="178" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" s="177"/>
+      <c r="E63" s="177"/>
+      <c r="F63" s="177"/>
+      <c r="G63" s="177"/>
+      <c r="H63" s="177"/>
+      <c r="I63" s="177"/>
+      <c r="J63" s="177"/>
+      <c r="K63" s="177"/>
+      <c r="L63" s="177"/>
+      <c r="M63" s="177"/>
+      <c r="N63" s="177"/>
+      <c r="O63" s="177"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B64" s="178" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="178" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" s="177"/>
+      <c r="E64" s="177"/>
+      <c r="F64" s="177"/>
+      <c r="G64" s="177"/>
+      <c r="H64" s="177"/>
+      <c r="I64" s="177"/>
+      <c r="J64" s="177"/>
+      <c r="K64" s="177"/>
+      <c r="L64" s="177"/>
+      <c r="M64" s="177"/>
+      <c r="N64" s="177"/>
+      <c r="O64" s="177"/>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B65" s="178" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="178" t="s">
+        <v>72</v>
+      </c>
+      <c r="D65" s="177"/>
+      <c r="E65" s="177"/>
+      <c r="F65" s="177"/>
+      <c r="G65" s="177"/>
+      <c r="H65" s="177"/>
+      <c r="I65" s="177"/>
+      <c r="J65" s="177"/>
+      <c r="K65" s="177"/>
+      <c r="L65" s="177"/>
+      <c r="M65" s="177"/>
+      <c r="N65" s="177"/>
+      <c r="O65" s="177"/>
+    </row>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B66" s="178" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" s="178" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66" s="177"/>
+      <c r="E66" s="177"/>
+      <c r="F66" s="177"/>
+      <c r="G66" s="177"/>
+      <c r="H66" s="177"/>
+      <c r="I66" s="177"/>
+      <c r="J66" s="177"/>
+      <c r="K66" s="177"/>
+      <c r="L66" s="177"/>
+      <c r="M66" s="177"/>
+      <c r="N66" s="177"/>
+      <c r="O66" s="177"/>
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B67" s="178" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" s="178" t="s">
+        <v>74</v>
+      </c>
+      <c r="D67" s="177"/>
+      <c r="E67" s="177"/>
+      <c r="F67" s="177"/>
+      <c r="G67" s="177"/>
+      <c r="H67" s="177"/>
+      <c r="I67" s="177"/>
+      <c r="J67" s="177"/>
+      <c r="K67" s="177"/>
+      <c r="L67" s="177"/>
+      <c r="M67" s="177"/>
+      <c r="N67" s="177"/>
+      <c r="O67" s="177"/>
+    </row>
+    <row r="68" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B68" s="178" t="s">
+        <v>75</v>
+      </c>
+      <c r="C68" s="178" t="s">
+        <v>75</v>
+      </c>
+      <c r="D68" s="177"/>
+      <c r="E68" s="177"/>
+      <c r="F68" s="177"/>
+      <c r="G68" s="177"/>
+      <c r="H68" s="177"/>
+      <c r="I68" s="177"/>
+      <c r="J68" s="177"/>
+      <c r="K68" s="177"/>
+      <c r="L68" s="177"/>
+      <c r="M68" s="177"/>
+      <c r="N68" s="177"/>
+      <c r="O68" s="177"/>
+    </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B69" s="178" t="s">
+        <v>76</v>
+      </c>
+      <c r="C69" s="178" t="s">
+        <v>76</v>
+      </c>
+      <c r="D69" s="177"/>
+      <c r="E69" s="177"/>
+      <c r="F69" s="177"/>
+      <c r="G69" s="177"/>
+      <c r="H69" s="177"/>
+      <c r="I69" s="177"/>
+      <c r="J69" s="177"/>
+      <c r="K69" s="177"/>
+      <c r="L69" s="177"/>
+      <c r="M69" s="177"/>
+      <c r="N69" s="177"/>
+      <c r="O69" s="177"/>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B70" s="178" t="s">
+        <v>77</v>
+      </c>
+      <c r="C70" s="178" t="s">
+        <v>77</v>
+      </c>
+      <c r="D70" s="177"/>
+      <c r="E70" s="177"/>
+      <c r="F70" s="177"/>
+      <c r="G70" s="177"/>
+      <c r="H70" s="177"/>
+      <c r="I70" s="177"/>
+      <c r="J70" s="177"/>
+      <c r="K70" s="177"/>
+      <c r="L70" s="177"/>
+      <c r="M70" s="177"/>
+      <c r="N70" s="177"/>
+      <c r="O70" s="177"/>
+    </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B71" s="178" t="s">
+        <v>312</v>
+      </c>
+      <c r="C71" s="178" t="s">
+        <v>312</v>
+      </c>
+      <c r="D71" s="177"/>
+      <c r="E71" s="177"/>
+      <c r="F71" s="177"/>
+      <c r="G71" s="177"/>
+      <c r="H71" s="177"/>
+      <c r="I71" s="177"/>
+      <c r="J71" s="177"/>
+      <c r="K71" s="177"/>
+      <c r="L71" s="177"/>
+      <c r="M71" s="177"/>
+      <c r="N71" s="177"/>
+      <c r="O71" s="177"/>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B72" s="178" t="s">
+        <v>313</v>
+      </c>
+      <c r="C72" s="178" t="s">
+        <v>313</v>
+      </c>
+      <c r="D72" s="177"/>
+      <c r="E72" s="177"/>
+      <c r="F72" s="177"/>
+      <c r="G72" s="177"/>
+      <c r="H72" s="177"/>
+      <c r="I72" s="177"/>
+      <c r="J72" s="177"/>
+      <c r="K72" s="177"/>
+      <c r="L72" s="177"/>
+      <c r="M72" s="177"/>
+      <c r="N72" s="177"/>
+      <c r="O72" s="177"/>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B73" s="178" t="s">
+        <v>314</v>
+      </c>
+      <c r="C73" s="178" t="s">
+        <v>314</v>
+      </c>
+      <c r="D73" s="177"/>
+      <c r="E73" s="177"/>
+      <c r="F73" s="177"/>
+      <c r="G73" s="177"/>
+      <c r="H73" s="177"/>
+      <c r="I73" s="177"/>
+      <c r="J73" s="177"/>
+      <c r="K73" s="177"/>
+      <c r="L73" s="177"/>
+      <c r="M73" s="177"/>
+      <c r="N73" s="177"/>
+      <c r="O73" s="177"/>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B74" s="178" t="s">
+        <v>315</v>
+      </c>
+      <c r="C74" s="178" t="s">
+        <v>315</v>
+      </c>
+      <c r="D74" s="177"/>
+      <c r="E74" s="177"/>
+      <c r="F74" s="177"/>
+      <c r="G74" s="177"/>
+      <c r="H74" s="177"/>
+      <c r="I74" s="177"/>
+      <c r="J74" s="177"/>
+      <c r="K74" s="177"/>
+      <c r="L74" s="177"/>
+      <c r="M74" s="177"/>
+      <c r="N74" s="177"/>
+      <c r="O74" s="177"/>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B75" s="178" t="s">
+        <v>316</v>
+      </c>
+      <c r="C75" s="178" t="s">
+        <v>316</v>
+      </c>
+      <c r="D75" s="177"/>
+      <c r="E75" s="177"/>
+      <c r="F75" s="177"/>
+      <c r="G75" s="177"/>
+      <c r="H75" s="177"/>
+      <c r="I75" s="177"/>
+      <c r="J75" s="177"/>
+      <c r="K75" s="177"/>
+      <c r="L75" s="177"/>
+      <c r="M75" s="177"/>
+      <c r="N75" s="177"/>
+      <c r="O75" s="177"/>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B76" s="178" t="s">
+        <v>317</v>
+      </c>
+      <c r="C76" s="178" t="s">
+        <v>317</v>
+      </c>
+      <c r="D76" s="177"/>
+      <c r="E76" s="177"/>
+      <c r="F76" s="177"/>
+      <c r="G76" s="177"/>
+      <c r="H76" s="177"/>
+      <c r="I76" s="177"/>
+      <c r="J76" s="177"/>
+      <c r="K76" s="177"/>
+      <c r="L76" s="177"/>
+      <c r="M76" s="177"/>
+      <c r="N76" s="177"/>
+      <c r="O76" s="177"/>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B77" s="178" t="s">
+        <v>318</v>
+      </c>
+      <c r="C77" s="178" t="s">
+        <v>318</v>
+      </c>
+      <c r="D77" s="177"/>
+      <c r="E77" s="177"/>
+      <c r="F77" s="177"/>
+      <c r="G77" s="177"/>
+      <c r="H77" s="177"/>
+      <c r="I77" s="177"/>
+      <c r="J77" s="177"/>
+      <c r="K77" s="177"/>
+      <c r="L77" s="177"/>
+      <c r="M77" s="177"/>
+      <c r="N77" s="177"/>
+      <c r="O77" s="177"/>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B78" s="178" t="s">
+        <v>319</v>
+      </c>
+      <c r="C78" s="178" t="s">
+        <v>319</v>
+      </c>
+      <c r="D78" s="177"/>
+      <c r="E78" s="177"/>
+      <c r="F78" s="177"/>
+      <c r="G78" s="177"/>
+      <c r="H78" s="177"/>
+      <c r="I78" s="177"/>
+      <c r="J78" s="177"/>
+      <c r="K78" s="177"/>
+      <c r="L78" s="177"/>
+      <c r="M78" s="177"/>
+      <c r="N78" s="177"/>
+      <c r="O78" s="177"/>
+    </row>
+    <row r="79" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B79" s="178" t="s">
+        <v>320</v>
+      </c>
+      <c r="C79" s="178" t="s">
+        <v>320</v>
+      </c>
+      <c r="D79" s="177"/>
+      <c r="E79" s="177"/>
+      <c r="F79" s="177"/>
+      <c r="G79" s="177"/>
+      <c r="H79" s="177"/>
+      <c r="I79" s="177"/>
+      <c r="J79" s="177"/>
+      <c r="K79" s="177"/>
+      <c r="L79" s="177"/>
+      <c r="M79" s="177"/>
+      <c r="N79" s="177"/>
+      <c r="O79" s="177"/>
+    </row>
+    <row r="80" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B80" s="178" t="s">
+        <v>321</v>
+      </c>
+      <c r="C80" s="178" t="s">
+        <v>321</v>
+      </c>
+      <c r="D80" s="177"/>
+      <c r="E80" s="177"/>
+      <c r="F80" s="177"/>
+      <c r="G80" s="177"/>
+      <c r="H80" s="177"/>
+      <c r="I80" s="177"/>
+      <c r="J80" s="177"/>
+      <c r="K80" s="177"/>
+      <c r="L80" s="177"/>
+      <c r="M80" s="177"/>
+      <c r="N80" s="177"/>
+      <c r="O80" s="177"/>
+    </row>
+    <row r="81" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B81" s="178" t="s">
+        <v>322</v>
+      </c>
+      <c r="C81" s="178" t="s">
+        <v>322</v>
+      </c>
+      <c r="D81" s="177"/>
+      <c r="E81" s="177"/>
+      <c r="F81" s="177"/>
+      <c r="G81" s="177"/>
+      <c r="H81" s="177"/>
+      <c r="I81" s="177"/>
+      <c r="J81" s="177"/>
+      <c r="K81" s="177"/>
+      <c r="L81" s="177"/>
+      <c r="M81" s="177"/>
+      <c r="N81" s="177"/>
+      <c r="O81" s="177"/>
+    </row>
+    <row r="82" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B82" s="178" t="s">
+        <v>323</v>
+      </c>
+      <c r="C82" s="178" t="s">
+        <v>323</v>
+      </c>
+      <c r="D82" s="177"/>
+      <c r="E82" s="177"/>
+      <c r="F82" s="177"/>
+      <c r="G82" s="177"/>
+      <c r="H82" s="177"/>
+      <c r="I82" s="177"/>
+      <c r="J82" s="177"/>
+      <c r="K82" s="177"/>
+      <c r="L82" s="177"/>
+      <c r="M82" s="177"/>
+      <c r="N82" s="177"/>
+      <c r="O82" s="177"/>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B83" s="178" t="s">
+        <v>324</v>
+      </c>
+      <c r="C83" s="178" t="s">
+        <v>324</v>
+      </c>
+      <c r="D83" s="177"/>
+      <c r="E83" s="177"/>
+      <c r="F83" s="177"/>
+      <c r="G83" s="177"/>
+      <c r="H83" s="177"/>
+      <c r="I83" s="177"/>
+      <c r="J83" s="177"/>
+      <c r="K83" s="177"/>
+      <c r="L83" s="177"/>
+      <c r="M83" s="177"/>
+      <c r="N83" s="177"/>
+      <c r="O83" s="177"/>
+    </row>
+    <row r="84" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B84" s="178" t="s">
+        <v>325</v>
+      </c>
+      <c r="C84" s="178" t="s">
+        <v>325</v>
+      </c>
+      <c r="D84" s="177"/>
+      <c r="E84" s="177"/>
+      <c r="F84" s="177"/>
+      <c r="G84" s="177"/>
+      <c r="H84" s="177"/>
+      <c r="I84" s="177"/>
+      <c r="J84" s="177"/>
+      <c r="K84" s="177"/>
+      <c r="L84" s="177"/>
+      <c r="M84" s="177"/>
+      <c r="N84" s="177"/>
+      <c r="O84" s="177"/>
+    </row>
+    <row r="85" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B85" s="178" t="s">
+        <v>326</v>
+      </c>
+      <c r="C85" s="178" t="s">
+        <v>326</v>
+      </c>
+      <c r="D85" s="177"/>
+      <c r="E85" s="177"/>
+      <c r="F85" s="177"/>
+      <c r="G85" s="177"/>
+      <c r="H85" s="177"/>
+      <c r="I85" s="177"/>
+      <c r="J85" s="177"/>
+      <c r="K85" s="177"/>
+      <c r="L85" s="177"/>
+      <c r="M85" s="177"/>
+      <c r="N85" s="177"/>
+      <c r="O85" s="177"/>
+    </row>
+    <row r="86" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B86" s="178" t="s">
+        <v>327</v>
+      </c>
+      <c r="C86" s="178" t="s">
+        <v>327</v>
+      </c>
+      <c r="D86" s="177"/>
+      <c r="E86" s="177"/>
+      <c r="F86" s="177"/>
+      <c r="G86" s="177"/>
+      <c r="H86" s="177"/>
+      <c r="I86" s="177"/>
+      <c r="J86" s="177"/>
+      <c r="K86" s="177"/>
+      <c r="L86" s="177"/>
+      <c r="M86" s="177"/>
+      <c r="N86" s="177"/>
+      <c r="O86" s="177"/>
+    </row>
+    <row r="87" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B87" s="178" t="s">
+        <v>328</v>
+      </c>
+      <c r="C87" s="178" t="s">
+        <v>328</v>
+      </c>
+      <c r="D87" s="177"/>
+      <c r="E87" s="177"/>
+      <c r="F87" s="177"/>
+      <c r="G87" s="177"/>
+      <c r="H87" s="177"/>
+      <c r="I87" s="177"/>
+      <c r="J87" s="177"/>
+      <c r="K87" s="177"/>
+      <c r="L87" s="177"/>
+      <c r="M87" s="177"/>
+      <c r="N87" s="177"/>
+      <c r="O87" s="177"/>
+    </row>
+    <row r="88" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B88" s="178" t="s">
+        <v>329</v>
+      </c>
+      <c r="C88" s="178" t="s">
+        <v>329</v>
+      </c>
+      <c r="D88" s="177"/>
+      <c r="E88" s="177"/>
+      <c r="F88" s="177"/>
+      <c r="G88" s="177"/>
+      <c r="H88" s="177"/>
+      <c r="I88" s="177"/>
+      <c r="J88" s="177"/>
+      <c r="K88" s="177"/>
+      <c r="L88" s="177"/>
+      <c r="M88" s="177"/>
+      <c r="N88" s="177"/>
+      <c r="O88" s="177"/>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B89" s="178" t="s">
+        <v>330</v>
+      </c>
+      <c r="C89" s="178" t="s">
+        <v>330</v>
+      </c>
+      <c r="D89" s="177"/>
+      <c r="E89" s="177"/>
+      <c r="F89" s="177"/>
+      <c r="G89" s="177"/>
+      <c r="H89" s="177"/>
+      <c r="I89" s="177"/>
+      <c r="J89" s="177"/>
+      <c r="K89" s="177"/>
+      <c r="L89" s="177"/>
+      <c r="M89" s="177"/>
+      <c r="N89" s="177"/>
+      <c r="O89" s="177"/>
+    </row>
+    <row r="90" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B90" s="178" t="s">
+        <v>331</v>
+      </c>
+      <c r="C90" s="178" t="s">
+        <v>331</v>
+      </c>
+      <c r="D90" s="177"/>
+      <c r="E90" s="177"/>
+      <c r="F90" s="177"/>
+      <c r="G90" s="177"/>
+      <c r="H90" s="177"/>
+      <c r="I90" s="177"/>
+      <c r="J90" s="177"/>
+      <c r="K90" s="177"/>
+      <c r="L90" s="177"/>
+      <c r="M90" s="177"/>
+      <c r="N90" s="177"/>
+      <c r="O90" s="177"/>
+    </row>
+    <row r="91" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B91" s="178" t="s">
+        <v>332</v>
+      </c>
+      <c r="C91" s="178" t="s">
+        <v>332</v>
+      </c>
+      <c r="D91" s="177"/>
+      <c r="E91" s="177"/>
+      <c r="F91" s="177"/>
+      <c r="G91" s="177"/>
+      <c r="H91" s="177"/>
+      <c r="I91" s="177"/>
+      <c r="J91" s="177"/>
+      <c r="K91" s="177"/>
+      <c r="L91" s="177"/>
+      <c r="M91" s="177"/>
+      <c r="N91" s="177"/>
+      <c r="O91" s="177"/>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B92" s="178" t="s">
+        <v>333</v>
+      </c>
+      <c r="C92" s="178" t="s">
+        <v>333</v>
+      </c>
+      <c r="D92" s="177"/>
+      <c r="E92" s="177"/>
+      <c r="F92" s="177"/>
+      <c r="G92" s="177"/>
+      <c r="H92" s="177"/>
+      <c r="I92" s="177"/>
+      <c r="J92" s="177"/>
+      <c r="K92" s="177"/>
+      <c r="L92" s="177"/>
+      <c r="M92" s="177"/>
+      <c r="N92" s="177"/>
+      <c r="O92" s="177"/>
+    </row>
+    <row r="93" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B93" s="178" t="s">
+        <v>334</v>
+      </c>
+      <c r="C93" s="178" t="s">
+        <v>334</v>
+      </c>
+      <c r="D93" s="177"/>
+      <c r="E93" s="177"/>
+      <c r="F93" s="177"/>
+      <c r="G93" s="177"/>
+      <c r="H93" s="177"/>
+      <c r="I93" s="177"/>
+      <c r="J93" s="177"/>
+      <c r="K93" s="177"/>
+      <c r="L93" s="177"/>
+      <c r="M93" s="177"/>
+      <c r="N93" s="177"/>
+      <c r="O93" s="177"/>
+    </row>
+    <row r="94" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B94" s="178" t="s">
+        <v>335</v>
+      </c>
+      <c r="C94" s="178" t="s">
+        <v>335</v>
+      </c>
+      <c r="D94" s="177"/>
+      <c r="E94" s="177"/>
+      <c r="F94" s="177"/>
+      <c r="G94" s="177"/>
+      <c r="H94" s="177"/>
+      <c r="I94" s="177"/>
+      <c r="J94" s="177"/>
+      <c r="K94" s="177"/>
+      <c r="L94" s="177"/>
+      <c r="M94" s="177"/>
+      <c r="N94" s="177"/>
+      <c r="O94" s="177"/>
+    </row>
+    <row r="95" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B95" s="178" t="s">
+        <v>336</v>
+      </c>
+      <c r="C95" s="178" t="s">
+        <v>336</v>
+      </c>
+      <c r="D95" s="177"/>
+      <c r="E95" s="177"/>
+      <c r="F95" s="177"/>
+      <c r="G95" s="177"/>
+      <c r="H95" s="177"/>
+      <c r="I95" s="177"/>
+      <c r="J95" s="177"/>
+      <c r="K95" s="177"/>
+      <c r="L95" s="177"/>
+      <c r="M95" s="177"/>
+      <c r="N95" s="177"/>
+      <c r="O95" s="177"/>
+    </row>
+    <row r="96" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B96" s="178" t="s">
+        <v>337</v>
+      </c>
+      <c r="C96" s="178" t="s">
+        <v>337</v>
+      </c>
+      <c r="D96" s="177"/>
+      <c r="E96" s="177"/>
+      <c r="F96" s="177"/>
+      <c r="G96" s="177"/>
+      <c r="H96" s="177"/>
+      <c r="I96" s="177"/>
+      <c r="J96" s="177"/>
+      <c r="K96" s="177"/>
+      <c r="L96" s="177"/>
+      <c r="M96" s="177"/>
+      <c r="N96" s="177"/>
+      <c r="O96" s="177"/>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B97" s="178" t="s">
+        <v>338</v>
+      </c>
+      <c r="C97" s="178" t="s">
+        <v>338</v>
+      </c>
+      <c r="D97" s="177"/>
+      <c r="E97" s="177"/>
+      <c r="F97" s="177"/>
+      <c r="G97" s="177"/>
+      <c r="H97" s="177"/>
+      <c r="I97" s="177"/>
+      <c r="J97" s="177"/>
+      <c r="K97" s="177"/>
+      <c r="L97" s="177"/>
+      <c r="M97" s="177"/>
+      <c r="N97" s="177"/>
+      <c r="O97" s="177"/>
+    </row>
+    <row r="98" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B98" s="178" t="s">
+        <v>339</v>
+      </c>
+      <c r="C98" s="178" t="s">
+        <v>339</v>
+      </c>
+      <c r="D98" s="177"/>
+      <c r="E98" s="177"/>
+      <c r="F98" s="177"/>
+      <c r="G98" s="177"/>
+      <c r="H98" s="177"/>
+      <c r="I98" s="177"/>
+      <c r="J98" s="177"/>
+      <c r="K98" s="177"/>
+      <c r="L98" s="177"/>
+      <c r="M98" s="177"/>
+      <c r="N98" s="177"/>
+      <c r="O98" s="177"/>
+    </row>
+    <row r="99" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B99" s="178" t="s">
+        <v>340</v>
+      </c>
+      <c r="C99" s="178" t="s">
+        <v>340</v>
+      </c>
+      <c r="D99" s="177"/>
+      <c r="E99" s="177"/>
+      <c r="F99" s="177"/>
+      <c r="G99" s="177"/>
+      <c r="H99" s="177"/>
+      <c r="I99" s="177"/>
+      <c r="J99" s="177"/>
+      <c r="K99" s="177"/>
+      <c r="L99" s="177"/>
+      <c r="M99" s="177"/>
+      <c r="N99" s="177"/>
+      <c r="O99" s="177"/>
+    </row>
+    <row r="100" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B100" s="177"/>
+      <c r="C100" s="177"/>
+      <c r="D100" s="177"/>
+      <c r="E100" s="177"/>
+      <c r="F100" s="177"/>
+      <c r="G100" s="177"/>
+      <c r="H100" s="177"/>
+      <c r="I100" s="177"/>
+      <c r="J100" s="177"/>
+      <c r="K100" s="177"/>
+      <c r="L100" s="177"/>
+      <c r="M100" s="177"/>
+      <c r="N100" s="177"/>
+      <c r="O100" s="177"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="G6:I6"/>
@@ -28470,8 +29809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{224FCEC0-8C66-41AA-B60E-F73836411637}">
   <dimension ref="B2:AB112"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81:W81"/>
+    <sheetView showGridLines="0" topLeftCell="A83" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33874,7 +35213,7 @@
         <v>126</v>
       </c>
       <c r="P94" s="75" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q94" s="74" t="s">
         <v>127</v>
@@ -34054,7 +35393,7 @@
       </c>
       <c r="P96" s="86">
         <f t="shared" si="32"/>
-        <v>1580.5938864628824</v>
+        <v>1762.5327510917032</v>
       </c>
       <c r="Q96" s="104">
         <f t="shared" si="32"/>
@@ -34141,7 +35480,7 @@
       <c r="N97" s="152"/>
       <c r="O97" s="151">
         <f>(MAX(O96:P96)-MIN(O96:P96))/(MAX(O96:P96))</f>
-        <v>0</v>
+        <v>0.10322580645161276</v>
       </c>
       <c r="P97" s="152"/>
       <c r="Q97" s="151">
@@ -34211,7 +35550,7 @@
       <c r="N98" s="154"/>
       <c r="O98" s="153">
         <f>IF(O97&lt;25%,(O96*0.5+P96*0.5)*0.9,IF(O97&lt;50%,(MAX(O96:P96)*0.6+MIN(O96:P96)*0.4)*0.9,IF(O97&lt;70%,(MAX(O96:P96)*0.65+MIN(O96:P96)*0.35)*0.9,IF(O97&lt;100%,(MAX(O96:P96)*0.7+MIN(O96:P96)*0.3)*0.9,0.7*MAX(O96:P96)))))</f>
-        <v>1422.5344978165942</v>
+        <v>1504.4069868995637</v>
       </c>
       <c r="P98" s="154"/>
       <c r="Q98" s="153">
@@ -34281,7 +35620,7 @@
       <c r="N99" s="144"/>
       <c r="O99" s="143">
         <f>O98/(0.9*(0.9*($C$7/100))*($L$9*1000))</f>
-        <v>2.9309336271749036</v>
+        <v>3.0996204546382073</v>
       </c>
       <c r="P99" s="144"/>
       <c r="Q99" s="143">
@@ -34351,7 +35690,7 @@
       <c r="N100" s="146"/>
       <c r="O100" s="145">
         <f>(O99*($L$9))/(0.85*$L$6*100)</f>
-        <v>4.1339251686632356E-2</v>
+        <v>4.3718489193776661E-2</v>
       </c>
       <c r="P100" s="146"/>
       <c r="Q100" s="145">
@@ -34421,7 +35760,7 @@
       <c r="N101" s="148"/>
       <c r="O101" s="147">
         <f>ROUNDUP(O98/(0.9*(($C$7-O100/2)/100)*($L$9*1000)),2)</f>
-        <v>2.65</v>
+        <v>2.8</v>
       </c>
       <c r="P101" s="148"/>
       <c r="Q101" s="147">
@@ -34504,11 +35843,11 @@
         <v>φ10@18</v>
       </c>
       <c r="T102" s="150"/>
-      <c r="U102" s="149" t="str">
+      <c r="U102" s="181" t="str">
         <f>IF(U101&gt;$C$12,"φ"&amp;IF(VLOOKUP(VLOOKUP(U101,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(U101,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;U101,VLOOKUP(U101+0.1,tablas!$R$3:$T$66,2,TRUE),VLOOKUP(U101,tablas!$R$3:$T$66,2,TRUE))&amp;"@"&amp;IF(VLOOKUP(VLOOKUP(U101,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(U101,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;U101,VLOOKUP(U101+0.1,tablas!$R$3:$T$66,3,TRUE),VLOOKUP(U101,tablas!$R$3:$T$66,3,TRUE)),$C$13)</f>
         <v>φ8@13</v>
       </c>
-      <c r="V102" s="150"/>
+      <c r="V102" s="182"/>
       <c r="W102" s="149" t="str">
         <f>IF(W101&gt;$C$12,"φ"&amp;IF(VLOOKUP(VLOOKUP(W101,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(W101,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;W101,VLOOKUP(W101+0.1,tablas!$R$3:$T$66,2,TRUE),VLOOKUP(W101,tablas!$R$3:$T$66,2,TRUE))&amp;"@"&amp;IF(VLOOKUP(VLOOKUP(W101,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(W101,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;W101,VLOOKUP(W101+0.1,tablas!$R$3:$T$66,3,TRUE),VLOOKUP(W101,tablas!$R$3:$T$66,3,TRUE)),$C$13)</f>
         <v>φ12@20</v>
@@ -35069,11 +36408,11 @@
       <c r="B112" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="C112" s="149" t="str">
+      <c r="C112" s="181" t="str">
         <f>IF(C111&gt;$C$12,"φ"&amp;IF(VLOOKUP(VLOOKUP(C111,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(C111,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;C111,VLOOKUP(C111+0.1,tablas!$R$3:$T$66,2,TRUE),VLOOKUP(C111,tablas!$R$3:$T$66,2,TRUE))&amp;"@"&amp;IF(VLOOKUP(VLOOKUP(C111,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(C111,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;C111,VLOOKUP(C111+0.1,tablas!$R$3:$T$66,3,TRUE),VLOOKUP(C111,tablas!$R$3:$T$66,3,TRUE)),$C$13)</f>
         <v>φ8@17</v>
       </c>
-      <c r="D112" s="150"/>
+      <c r="D112" s="182"/>
       <c r="E112" s="149" t="str">
         <f>IF(E111&gt;$C$12,"φ"&amp;IF(VLOOKUP(VLOOKUP(E111,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(E111,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;E111,VLOOKUP(E111+0.1,tablas!$R$3:$T$66,2,TRUE),VLOOKUP(E111,tablas!$R$3:$T$66,2,TRUE))&amp;"@"&amp;IF(VLOOKUP(VLOOKUP(E111,tablas!$R$3:$T$66,2,TRUE)&amp;VLOOKUP(E111,tablas!$R$3:$T$66,3,TRUE),tablas!$Q$3:$R$66,2,FALSE)&lt;E111,VLOOKUP(E111+0.1,tablas!$R$3:$T$66,3,TRUE),VLOOKUP(E111,tablas!$R$3:$T$66,3,TRUE)),$C$13)</f>
         <v>φ8@17</v>
@@ -36222,8 +37561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64344204-6196-4517-B7F8-8D15C521CC45}">
   <dimension ref="B2:Z113"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="L53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82:X82"/>
+    <sheetView showGridLines="0" topLeftCell="I79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S113" sqref="S113:T113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57561,7 +58900,7 @@
   <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:L27"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>